<commit_message>
updated biofuels and a group of other things
</commit_message>
<xml_diff>
--- a/config/biofuel_capacity_parameters.xlsx
+++ b/config/biofuel_capacity_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9655D2B5-35CE-4D72-AC2A-F31C0EA6AA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C54A23-D8F6-46A0-8650-055FC771AEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">simplified_economy_fuels!$A$1:$C$226</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,13 +74,14 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>Explanation of Methods:
+          <t xml:space="preserve">Explanation of Methods:
+-do_nothing : will do nothing. Ideal if you wat complete control over capcity. 
 - satisfy_all_demand_with_domestic_production:
-    The economy satisfies all demand for a fuel with domestic production. This eliminates imports and exports, making the economy self-sufficient.
+    The economy satisfies all demand for a fuel with domestic production. This eliminates imports and exports, making the economy self-sufficient.. If working with a series that has already had capcaity data entered in (through ##_ECONOMY_capacity sheet), the code only adjusts prodcution if its LESS THAN CONSUMPTION. If the capacity that is recorded is more than consumption then it will jsut mean there are exports. 
 - satisfy_all_demand_with_domestic_production_RAMP:
-    Gradually increases domestic production over time to meet 100% of demand, avoiding sudden jumps in production.
+    Gradually increases domestic production over time to meet 100% of demand, avoiding sudden jumps in production. If working with a series that has already had capcaity data entered in (through ##_ECONOMY_capacity sheet), the code only adjusts prodcution if its LESS THAN CONSUMPTION. If the capacity that is recorded is more than consumption then it will jsut mean there are exports. 
 - keep_same_ratio_of_production_to_consumption:
-    Maintains the existing ratio of exports, imports, and production, while ensuring all demand is met with domestic production.</t>
+    Maintains the existing ratio of exports, imports, and production, while ensuring all demand is met with domestic production. If working with a series that has already had capcaity data entered in (through ##_ECONOMY_capacity sheet), the code will throw an error because it would otherwise overwrite that data to make the ratio of production to consumption the same for all years. </t>
         </r>
       </text>
     </comment>
@@ -76,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="57">
   <si>
     <t>EBT_biofuels_list</t>
   </si>
@@ -245,6 +259,9 @@
   <si>
     <t>other_biomass</t>
   </si>
+  <si>
+    <t>do_nothing</t>
+  </si>
 </sst>
 </file>
 
@@ -262,6 +279,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,11 +317,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,7 +627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1455,9 +1476,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1483,22 +1506,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.3869907539859128</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2">
-        <v>2022</v>
+        <v>48</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2023</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1506,10 +1529,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2.1225694700972362</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -1517,328 +1540,128 @@
       <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="F3">
-        <v>2022</v>
+      <c r="F3" s="2">
+        <v>2024</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2.0263218139073729</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4">
-        <v>2022</v>
+        <v>48</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2025</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6.4334279185486025</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <v>2022</v>
+        <v>48</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2026</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>6.3814671262608726</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6">
-        <v>2022</v>
+        <v>48</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2027</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>7.2043774337811719</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7">
-        <v>2022</v>
+        <v>48</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2023</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>7.0805281123867445</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8">
-        <v>2022</v>
+        <v>48</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2024</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>5.0658715366320806</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="F12">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19">
-        <v>2022</v>
+      <c r="F9" s="2">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>
@@ -6903,8 +6726,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="A226" sqref="A226"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6964,7 +6787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -6975,7 +6798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6986,7 +6809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -6997,7 +6820,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -7008,7 +6831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -7019,7 +6842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -7030,7 +6853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -7041,7 +6864,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -7063,7 +6886,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -7074,7 +6897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -7085,7 +6908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -7096,7 +6919,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -7107,7 +6930,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -7118,7 +6941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -7129,7 +6952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -7140,7 +6963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -7151,7 +6974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -7162,7 +6985,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -7173,7 +6996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -7184,7 +7007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -7239,7 +7062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -7250,7 +7073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -7261,7 +7084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -7272,7 +7095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -7283,7 +7106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -7294,7 +7117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -7305,7 +7128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -7316,7 +7139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -7335,10 +7158,10 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -7349,7 +7172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -7360,7 +7183,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -7371,7 +7194,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -7382,7 +7205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -7393,7 +7216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -7404,7 +7227,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -7415,7 +7238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -7426,7 +7249,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -7437,7 +7260,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -7448,7 +7271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -7459,7 +7282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -7514,7 +7337,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -7525,7 +7348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -7536,7 +7359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -7547,7 +7370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -7558,7 +7381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>27</v>
       </c>
@@ -7569,7 +7392,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>28</v>
       </c>
@@ -7580,7 +7403,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>29</v>
       </c>
@@ -7591,7 +7414,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>30</v>
       </c>
@@ -7613,7 +7436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>32</v>
       </c>
@@ -7624,7 +7447,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>33</v>
       </c>
@@ -7635,7 +7458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -7646,7 +7469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>35</v>
       </c>
@@ -7657,7 +7480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -7668,7 +7491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>37</v>
       </c>
@@ -7679,7 +7502,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -7690,7 +7513,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -7701,7 +7524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -7712,7 +7535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>41</v>
       </c>
@@ -7723,7 +7546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>42</v>
       </c>
@@ -7734,7 +7557,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -7789,7 +7612,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -7800,7 +7623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -7811,7 +7634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>25</v>
       </c>
@@ -7822,7 +7645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -7833,7 +7656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>27</v>
       </c>
@@ -7844,7 +7667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>28</v>
       </c>
@@ -7855,7 +7678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -7866,7 +7689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>30</v>
       </c>
@@ -7888,7 +7711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>32</v>
       </c>
@@ -7899,7 +7722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>33</v>
       </c>
@@ -7910,7 +7733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>34</v>
       </c>
@@ -7921,7 +7744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>35</v>
       </c>
@@ -7932,7 +7755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -7943,7 +7766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>37</v>
       </c>
@@ -7954,7 +7777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>38</v>
       </c>
@@ -7965,7 +7788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>39</v>
       </c>
@@ -7976,7 +7799,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>40</v>
       </c>
@@ -7987,7 +7810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>41</v>
       </c>
@@ -7998,7 +7821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>42</v>
       </c>
@@ -8009,7 +7832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>43</v>
       </c>
@@ -8064,7 +7887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>15</v>
       </c>
@@ -8075,7 +7898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -8086,7 +7909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>25</v>
       </c>
@@ -8097,7 +7920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>26</v>
       </c>
@@ -8108,7 +7931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>27</v>
       </c>
@@ -8119,7 +7942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>28</v>
       </c>
@@ -8130,7 +7953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>29</v>
       </c>
@@ -8141,7 +7964,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>30</v>
       </c>
@@ -8163,7 +7986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>32</v>
       </c>
@@ -8174,7 +7997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>33</v>
       </c>
@@ -8185,7 +8008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>34</v>
       </c>
@@ -8196,7 +8019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>35</v>
       </c>
@@ -8207,7 +8030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>36</v>
       </c>
@@ -8218,7 +8041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>37</v>
       </c>
@@ -8229,7 +8052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>38</v>
       </c>
@@ -8240,7 +8063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -8251,7 +8074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>40</v>
       </c>
@@ -8262,7 +8085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>41</v>
       </c>
@@ -8273,7 +8096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>42</v>
       </c>
@@ -8284,7 +8107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>43</v>
       </c>
@@ -8339,7 +8162,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>15</v>
       </c>
@@ -8350,7 +8173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>24</v>
       </c>
@@ -8361,7 +8184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>25</v>
       </c>
@@ -8372,7 +8195,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>26</v>
       </c>
@@ -8383,7 +8206,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>27</v>
       </c>
@@ -8394,7 +8217,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>28</v>
       </c>
@@ -8405,7 +8228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>29</v>
       </c>
@@ -8416,7 +8239,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -8438,7 +8261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>32</v>
       </c>
@@ -8449,7 +8272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>33</v>
       </c>
@@ -8460,7 +8283,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>34</v>
       </c>
@@ -8471,7 +8294,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>35</v>
       </c>
@@ -8482,7 +8305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>36</v>
       </c>
@@ -8493,7 +8316,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>37</v>
       </c>
@@ -8504,7 +8327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>38</v>
       </c>
@@ -8515,7 +8338,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>39</v>
       </c>
@@ -8526,7 +8349,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>40</v>
       </c>
@@ -8537,7 +8360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>41</v>
       </c>
@@ -8548,7 +8371,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>42</v>
       </c>
@@ -8559,7 +8382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>43</v>
       </c>
@@ -8614,7 +8437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>15</v>
       </c>
@@ -8625,7 +8448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>24</v>
       </c>
@@ -8636,7 +8459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>25</v>
       </c>
@@ -8647,7 +8470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>26</v>
       </c>
@@ -8658,7 +8481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>27</v>
       </c>
@@ -8669,7 +8492,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>28</v>
       </c>
@@ -8680,7 +8503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>29</v>
       </c>
@@ -8691,7 +8514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>30</v>
       </c>
@@ -8713,7 +8536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>32</v>
       </c>
@@ -8724,7 +8547,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>33</v>
       </c>
@@ -8735,7 +8558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>34</v>
       </c>
@@ -8746,7 +8569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>35</v>
       </c>
@@ -8757,7 +8580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>36</v>
       </c>
@@ -8768,7 +8591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>37</v>
       </c>
@@ -8779,7 +8602,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>38</v>
       </c>
@@ -8790,7 +8613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>39</v>
       </c>
@@ -8801,7 +8624,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>40</v>
       </c>
@@ -8812,7 +8635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>41</v>
       </c>
@@ -8823,7 +8646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>42</v>
       </c>
@@ -8834,7 +8657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>43</v>
       </c>
@@ -8889,7 +8712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>15</v>
       </c>
@@ -8900,7 +8723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>24</v>
       </c>
@@ -8911,7 +8734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>25</v>
       </c>
@@ -8922,7 +8745,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>26</v>
       </c>
@@ -8933,7 +8756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>27</v>
       </c>
@@ -8944,7 +8767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>28</v>
       </c>
@@ -8955,7 +8778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>29</v>
       </c>
@@ -8966,7 +8789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>30</v>
       </c>
@@ -8988,7 +8811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>32</v>
       </c>
@@ -8999,7 +8822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>33</v>
       </c>
@@ -9010,7 +8833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>34</v>
       </c>
@@ -9021,7 +8844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>35</v>
       </c>
@@ -9032,7 +8855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>36</v>
       </c>
@@ -9043,7 +8866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>37</v>
       </c>
@@ -9054,7 +8877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>38</v>
       </c>
@@ -9065,7 +8888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>39</v>
       </c>
@@ -9076,7 +8899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>40</v>
       </c>
@@ -9087,7 +8910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>41</v>
       </c>
@@ -9098,7 +8921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>42</v>
       </c>
@@ -9109,7 +8932,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>43</v>
       </c>
@@ -9164,7 +8987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>15</v>
       </c>
@@ -9175,7 +8998,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>24</v>
       </c>
@@ -9186,7 +9009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>25</v>
       </c>
@@ -9197,7 +9020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>26</v>
       </c>
@@ -9208,7 +9031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>27</v>
       </c>
@@ -9219,7 +9042,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>28</v>
       </c>
@@ -9230,7 +9053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>29</v>
       </c>
@@ -9241,7 +9064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>30</v>
       </c>
@@ -9263,7 +9086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>32</v>
       </c>
@@ -9274,7 +9097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>33</v>
       </c>
@@ -9285,7 +9108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>34</v>
       </c>
@@ -9296,7 +9119,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>35</v>
       </c>
@@ -9307,7 +9130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>36</v>
       </c>
@@ -9318,7 +9141,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>37</v>
       </c>
@@ -9329,7 +9152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>38</v>
       </c>
@@ -9340,7 +9163,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>39</v>
       </c>
@@ -9351,7 +9174,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>40</v>
       </c>
@@ -9362,7 +9185,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>41</v>
       </c>
@@ -9373,7 +9196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>42</v>
       </c>
@@ -9384,7 +9207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>43</v>
       </c>
@@ -9399,37 +9222,13 @@
   <autoFilter ref="A1:C226" xr:uid="{00000000-0001-0000-0200-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="01_AUS"/>
-        <filter val="02_BD"/>
-        <filter val="03_CDA"/>
-        <filter val="04_CHL"/>
-        <filter val="05_PRC"/>
-        <filter val="06_HKC"/>
-        <filter val="07_INA"/>
-        <filter val="08_JPN"/>
         <filter val="09_ROK"/>
-        <filter val="10_MAS"/>
-        <filter val="11_MEX"/>
-        <filter val="12_NZ"/>
-        <filter val="13_PNG"/>
-        <filter val="14_PE"/>
-        <filter val="15_PHL"/>
-        <filter val="16_RUS"/>
-        <filter val="17_SGP"/>
-        <filter val="18_CT"/>
-        <filter val="19_THA"/>
-        <filter val="20_USA"/>
-        <filter val="21_VN"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="keep_same_ratio_of_production_to_consumption"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9437,9 +9236,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -9828,11 +9634,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="31.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -10213,6 +10024,30 @@
       <c r="F19">
         <v>2022</v>
       </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updates to handle 16_others and 15_solid better
</commit_message>
<xml_diff>
--- a/config/biofuel_capacity_parameters.xlsx
+++ b/config/biofuel_capacity_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1C2C83-4C49-4A93-8CB0-4E6BE195C284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A3A7BA-D142-4A90-8587-BB73526E55C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <sheet name="21_VN_capacity" sheetId="24" r:id="rId25"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">simplified_economy_fuels!$A$1:$C$353</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">simplified_economy_fuels!$A$1:$C$309</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="64">
   <si>
     <t>EBT_biofuels_list</t>
   </si>
@@ -285,12 +285,6 @@
   </si>
   <si>
     <t>16_08_other_liquid_biofuels</t>
-  </si>
-  <si>
-    <t>15_solid_biomass_x</t>
-  </si>
-  <si>
-    <t>16_others_x</t>
   </si>
 </sst>
 </file>
@@ -767,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,14 +841,10 @@
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="A15" s="5"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="A16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7334,10 +7324,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F353"/>
+  <dimension ref="A1:F309"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7373,172 +7363,172 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>63</v>
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>64</v>
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>65</v>
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -7549,10 +7539,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
         <v>57</v>
@@ -7560,10 +7550,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
@@ -7571,10 +7561,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
@@ -7582,10 +7572,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>57</v>
@@ -7593,10 +7583,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
         <v>57</v>
@@ -7604,13 +7594,13 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -7618,7 +7608,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>57</v>
@@ -7626,10 +7616,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>57</v>
@@ -7637,10 +7627,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
       </c>
       <c r="C27" t="s">
         <v>57</v>
@@ -7648,10 +7638,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>60</v>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>57</v>
@@ -7659,10 +7649,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>61</v>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
       </c>
       <c r="C29" t="s">
         <v>57</v>
@@ -7670,10 +7660,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>63</v>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>57</v>
@@ -7681,10 +7671,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>62</v>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>57</v>
@@ -7692,10 +7682,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>64</v>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
       </c>
       <c r="C32" t="s">
         <v>57</v>
@@ -7703,10 +7693,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>65</v>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
       </c>
       <c r="C33" t="s">
         <v>57</v>
@@ -7714,10 +7704,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
         <v>57</v>
@@ -7725,7 +7715,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -7736,10 +7726,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
@@ -7747,10 +7737,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
         <v>57</v>
@@ -7758,10 +7748,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
         <v>57</v>
@@ -7769,10 +7759,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
         <v>57</v>
@@ -7780,10 +7770,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
         <v>57</v>
@@ -7791,10 +7781,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
         <v>57</v>
@@ -7802,10 +7792,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
         <v>57</v>
@@ -7813,10 +7803,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>59</v>
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
       </c>
       <c r="C43" t="s">
         <v>57</v>
@@ -7824,10 +7814,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>60</v>
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
       </c>
       <c r="C44" t="s">
         <v>57</v>
@@ -7835,10 +7825,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
       </c>
       <c r="C45" t="s">
         <v>57</v>
@@ -7846,21 +7836,21 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>63</v>
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>62</v>
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
       </c>
       <c r="C47" t="s">
         <v>57</v>
@@ -7870,8 +7860,8 @@
       <c r="A48" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>64</v>
+      <c r="B48" t="s">
+        <v>7</v>
       </c>
       <c r="C48" t="s">
         <v>57</v>
@@ -7879,10 +7869,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>65</v>
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
       </c>
       <c r="C49" t="s">
         <v>57</v>
@@ -7890,10 +7880,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50" t="s">
         <v>57</v>
@@ -7901,10 +7891,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
         <v>57</v>
@@ -7912,7 +7902,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -7923,10 +7913,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>57</v>
@@ -7934,10 +7924,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
         <v>57</v>
@@ -7945,10 +7935,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
         <v>57</v>
@@ -7956,10 +7946,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
         <v>57</v>
@@ -7967,10 +7957,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
         <v>57</v>
@@ -7978,10 +7968,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
         <v>57</v>
@@ -7989,10 +7979,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>59</v>
+        <v>35</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
       </c>
       <c r="C59" t="s">
         <v>57</v>
@@ -8000,10 +7990,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>60</v>
+        <v>36</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
       </c>
       <c r="C60" t="s">
         <v>57</v>
@@ -8011,10 +8001,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
       </c>
       <c r="C61" t="s">
         <v>57</v>
@@ -8022,10 +8012,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>57</v>
@@ -8033,10 +8023,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>25</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
       </c>
       <c r="C63" t="s">
         <v>57</v>
@@ -8044,10 +8034,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>64</v>
+        <v>40</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
       </c>
       <c r="C64" t="s">
         <v>57</v>
@@ -8055,10 +8045,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>25</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>65</v>
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
       </c>
       <c r="C65" t="s">
         <v>57</v>
@@ -8066,10 +8056,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
         <v>57</v>
@@ -8077,10 +8067,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
         <v>57</v>
@@ -8088,18 +8078,18 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
@@ -8110,10 +8100,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70" t="s">
         <v>57</v>
@@ -8121,10 +8111,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
         <v>57</v>
@@ -8135,7 +8125,7 @@
         <v>26</v>
       </c>
       <c r="B72" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
         <v>57</v>
@@ -8143,10 +8133,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C73" t="s">
         <v>57</v>
@@ -8154,10 +8144,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
         <v>57</v>
@@ -8165,10 +8155,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>26</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>59</v>
+        <v>29</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
       </c>
       <c r="C75" t="s">
         <v>57</v>
@@ -8176,10 +8166,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>26</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>60</v>
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
       </c>
       <c r="C76" t="s">
         <v>57</v>
@@ -8187,10 +8177,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>26</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>61</v>
+        <v>31</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
       </c>
       <c r="C77" t="s">
         <v>57</v>
@@ -8198,10 +8188,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
       </c>
       <c r="C78" t="s">
         <v>57</v>
@@ -8209,10 +8199,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>26</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>62</v>
+        <v>33</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
       </c>
       <c r="C79" t="s">
         <v>57</v>
@@ -8220,10 +8210,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>26</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>64</v>
+        <v>34</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
       </c>
       <c r="C80" t="s">
         <v>57</v>
@@ -8231,10 +8221,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>26</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>65</v>
+        <v>35</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
       </c>
       <c r="C81" t="s">
         <v>57</v>
@@ -8242,10 +8232,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C82" t="s">
         <v>57</v>
@@ -8253,10 +8243,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
         <v>57</v>
@@ -8264,10 +8254,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C84" t="s">
         <v>57</v>
@@ -8275,7 +8265,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
@@ -8286,10 +8276,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
         <v>57</v>
@@ -8297,10 +8287,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C87" t="s">
         <v>57</v>
@@ -8308,10 +8298,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C88" t="s">
         <v>57</v>
@@ -8319,10 +8309,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B89" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C89" t="s">
         <v>57</v>
@@ -8330,21 +8320,21 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>27</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>59</v>
+        <v>15</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
       </c>
       <c r="C91" t="s">
         <v>57</v>
@@ -8352,10 +8342,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>27</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>60</v>
+        <v>24</v>
+      </c>
+      <c r="B92" t="s">
+        <v>9</v>
       </c>
       <c r="C92" t="s">
         <v>57</v>
@@ -8363,10 +8353,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>27</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>61</v>
+        <v>25</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
       </c>
       <c r="C93" t="s">
         <v>57</v>
@@ -8374,10 +8364,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>27</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>63</v>
+        <v>26</v>
+      </c>
+      <c r="B94" t="s">
+        <v>9</v>
       </c>
       <c r="C94" t="s">
         <v>57</v>
@@ -8387,8 +8377,8 @@
       <c r="A95" t="s">
         <v>27</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>62</v>
+      <c r="B95" t="s">
+        <v>9</v>
       </c>
       <c r="C95" t="s">
         <v>57</v>
@@ -8396,10 +8386,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>27</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>64</v>
+        <v>28</v>
+      </c>
+      <c r="B96" t="s">
+        <v>9</v>
       </c>
       <c r="C96" t="s">
         <v>57</v>
@@ -8407,10 +8397,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>27</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>65</v>
+        <v>29</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
       </c>
       <c r="C97" t="s">
         <v>57</v>
@@ -8418,10 +8408,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
         <v>57</v>
@@ -8429,10 +8419,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C99" t="s">
         <v>57</v>
@@ -8440,10 +8430,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C100" t="s">
         <v>57</v>
@@ -8451,10 +8441,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B101" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C101" t="s">
         <v>57</v>
@@ -8462,7 +8452,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
@@ -8473,10 +8463,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C103" t="s">
         <v>57</v>
@@ -8484,10 +8474,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B104" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C104" t="s">
         <v>57</v>
@@ -8495,10 +8485,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B105" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C105" t="s">
         <v>57</v>
@@ -8506,10 +8496,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B106" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C106" t="s">
         <v>57</v>
@@ -8517,10 +8507,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>28</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>59</v>
+        <v>39</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
       </c>
       <c r="C107" t="s">
         <v>57</v>
@@ -8528,10 +8518,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>28</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>60</v>
+        <v>40</v>
+      </c>
+      <c r="B108" t="s">
+        <v>9</v>
       </c>
       <c r="C108" t="s">
         <v>57</v>
@@ -8539,10 +8529,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>28</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>61</v>
+        <v>41</v>
+      </c>
+      <c r="B109" t="s">
+        <v>9</v>
       </c>
       <c r="C109" t="s">
         <v>57</v>
@@ -8550,10 +8540,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>28</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>63</v>
+        <v>42</v>
+      </c>
+      <c r="B110" t="s">
+        <v>9</v>
       </c>
       <c r="C110" t="s">
         <v>57</v>
@@ -8561,10 +8551,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>28</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>62</v>
+        <v>43</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
       </c>
       <c r="C111" t="s">
         <v>57</v>
@@ -8572,21 +8562,21 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>28</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>64</v>
+        <v>19</v>
+      </c>
+      <c r="B112" t="s">
+        <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>28</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>65</v>
+        <v>15</v>
+      </c>
+      <c r="B113" t="s">
+        <v>4</v>
       </c>
       <c r="C113" t="s">
         <v>57</v>
@@ -8594,10 +8584,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C114" t="s">
         <v>57</v>
@@ -8605,10 +8595,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C115" t="s">
         <v>57</v>
@@ -8616,10 +8606,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B116" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C116" t="s">
         <v>57</v>
@@ -8627,10 +8617,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B117" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C117" t="s">
         <v>57</v>
@@ -8638,10 +8628,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s">
         <v>57</v>
@@ -8660,10 +8650,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B120" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C120" t="s">
         <v>57</v>
@@ -8671,10 +8661,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B121" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C121" t="s">
         <v>57</v>
@@ -8682,10 +8672,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C122" t="s">
         <v>57</v>
@@ -8693,10 +8683,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>29</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>59</v>
+        <v>33</v>
+      </c>
+      <c r="B123" t="s">
+        <v>4</v>
       </c>
       <c r="C123" t="s">
         <v>57</v>
@@ -8704,10 +8694,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>29</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>60</v>
+        <v>34</v>
+      </c>
+      <c r="B124" t="s">
+        <v>4</v>
       </c>
       <c r="C124" t="s">
         <v>57</v>
@@ -8715,10 +8705,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>29</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>61</v>
+        <v>35</v>
+      </c>
+      <c r="B125" t="s">
+        <v>4</v>
       </c>
       <c r="C125" t="s">
         <v>57</v>
@@ -8726,10 +8716,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>29</v>
-      </c>
-      <c r="B126" s="6" t="s">
-        <v>63</v>
+        <v>36</v>
+      </c>
+      <c r="B126" t="s">
+        <v>4</v>
       </c>
       <c r="C126" t="s">
         <v>57</v>
@@ -8737,10 +8727,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>29</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="B127" t="s">
+        <v>4</v>
       </c>
       <c r="C127" t="s">
         <v>57</v>
@@ -8748,10 +8738,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>29</v>
-      </c>
-      <c r="B128" s="5" t="s">
-        <v>64</v>
+        <v>38</v>
+      </c>
+      <c r="B128" t="s">
+        <v>4</v>
       </c>
       <c r="C128" t="s">
         <v>57</v>
@@ -8759,10 +8749,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>29</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="B129" t="s">
+        <v>4</v>
       </c>
       <c r="C129" t="s">
         <v>57</v>
@@ -8770,10 +8760,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C130" t="s">
         <v>57</v>
@@ -8781,10 +8771,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B131" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C131" t="s">
         <v>57</v>
@@ -8792,10 +8782,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B132" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C132" t="s">
         <v>57</v>
@@ -8803,10 +8793,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B133" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C133" t="s">
         <v>57</v>
@@ -8814,21 +8804,21 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>30</v>
-      </c>
-      <c r="B134" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C134" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>30</v>
-      </c>
-      <c r="B135" t="s">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C135" t="s">
         <v>57</v>
@@ -8836,10 +8826,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>30</v>
-      </c>
-      <c r="B136" t="s">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C136" t="s">
         <v>57</v>
@@ -8847,10 +8837,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>30</v>
-      </c>
-      <c r="B137" t="s">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C137" t="s">
         <v>57</v>
@@ -8858,10 +8848,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>30</v>
-      </c>
-      <c r="B138" t="s">
-        <v>3</v>
+        <v>26</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C138" t="s">
         <v>57</v>
@@ -8869,7 +8859,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>59</v>
@@ -8880,10 +8870,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C140" t="s">
         <v>57</v>
@@ -8891,10 +8881,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C141" t="s">
         <v>57</v>
@@ -8905,7 +8895,7 @@
         <v>30</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C142" t="s">
         <v>57</v>
@@ -8913,10 +8903,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C143" t="s">
         <v>57</v>
@@ -8924,10 +8914,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>30</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>64</v>
+        <v>32</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C144" t="s">
         <v>57</v>
@@ -8935,10 +8925,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>30</v>
-      </c>
-      <c r="B145" s="5" t="s">
-        <v>65</v>
+        <v>33</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C145" t="s">
         <v>57</v>
@@ -8946,10 +8936,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>31</v>
-      </c>
-      <c r="B146" t="s">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C146" t="s">
         <v>57</v>
@@ -8957,10 +8947,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>31</v>
-      </c>
-      <c r="B147" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C147" t="s">
         <v>57</v>
@@ -8968,10 +8958,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>31</v>
-      </c>
-      <c r="B148" t="s">
-        <v>7</v>
+        <v>36</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C148" t="s">
         <v>57</v>
@@ -8979,10 +8969,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>31</v>
-      </c>
-      <c r="B149" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C149" t="s">
         <v>57</v>
@@ -8990,10 +8980,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>31</v>
-      </c>
-      <c r="B150" t="s">
-        <v>9</v>
+        <v>38</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C150" t="s">
         <v>57</v>
@@ -9001,10 +8991,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>31</v>
-      </c>
-      <c r="B151" t="s">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C151" t="s">
         <v>57</v>
@@ -9012,10 +9002,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>31</v>
-      </c>
-      <c r="B152" t="s">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C152" t="s">
         <v>57</v>
@@ -9023,10 +9013,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>31</v>
-      </c>
-      <c r="B153" t="s">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C153" t="s">
         <v>57</v>
@@ -9034,10 +9024,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>31</v>
-      </c>
-      <c r="B154" t="s">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C154" t="s">
         <v>57</v>
@@ -9045,7 +9035,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B155" s="6" t="s">
         <v>59</v>
@@ -9056,21 +9046,21 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C156" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C157" t="s">
         <v>57</v>
@@ -9078,10 +9068,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C158" t="s">
         <v>57</v>
@@ -9089,10 +9079,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C159" t="s">
         <v>57</v>
@@ -9100,10 +9090,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>31</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>64</v>
+        <v>26</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C160" t="s">
         <v>57</v>
@@ -9111,10 +9101,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>31</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>65</v>
+        <v>27</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C161" t="s">
         <v>57</v>
@@ -9122,10 +9112,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>32</v>
-      </c>
-      <c r="B162" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C162" t="s">
         <v>57</v>
@@ -9133,10 +9123,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>32</v>
-      </c>
-      <c r="B163" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C163" t="s">
         <v>57</v>
@@ -9144,10 +9134,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>32</v>
-      </c>
-      <c r="B164" t="s">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C164" t="s">
         <v>57</v>
@@ -9155,10 +9145,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>32</v>
-      </c>
-      <c r="B165" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C165" t="s">
         <v>57</v>
@@ -9168,8 +9158,8 @@
       <c r="A166" t="s">
         <v>32</v>
       </c>
-      <c r="B166" t="s">
-        <v>9</v>
+      <c r="B166" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C166" t="s">
         <v>57</v>
@@ -9177,10 +9167,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>32</v>
-      </c>
-      <c r="B167" t="s">
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C167" t="s">
         <v>57</v>
@@ -9188,10 +9178,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>32</v>
-      </c>
-      <c r="B168" t="s">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C168" t="s">
         <v>57</v>
@@ -9199,10 +9189,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>32</v>
-      </c>
-      <c r="B169" t="s">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C169" t="s">
         <v>57</v>
@@ -9210,10 +9200,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>32</v>
-      </c>
-      <c r="B170" t="s">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="B170" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C170" t="s">
         <v>57</v>
@@ -9221,10 +9211,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C171" t="s">
         <v>57</v>
@@ -9232,7 +9222,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>60</v>
@@ -9243,10 +9233,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C173" t="s">
         <v>57</v>
@@ -9254,10 +9244,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C174" t="s">
         <v>57</v>
@@ -9265,10 +9255,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C175" t="s">
         <v>57</v>
@@ -9276,10 +9266,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>32</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>64</v>
+        <v>42</v>
+      </c>
+      <c r="B176" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C176" t="s">
         <v>57</v>
@@ -9287,10 +9277,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>32</v>
-      </c>
-      <c r="B177" s="5" t="s">
-        <v>65</v>
+        <v>43</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C177" t="s">
         <v>57</v>
@@ -9298,21 +9288,21 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>33</v>
-      </c>
-      <c r="B178" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="B178" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C178" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>33</v>
-      </c>
-      <c r="B179" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C179" t="s">
         <v>57</v>
@@ -9320,10 +9310,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>33</v>
-      </c>
-      <c r="B180" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C180" t="s">
         <v>57</v>
@@ -9331,10 +9321,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>33</v>
-      </c>
-      <c r="B181" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C181" t="s">
         <v>57</v>
@@ -9342,10 +9332,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>33</v>
-      </c>
-      <c r="B182" t="s">
-        <v>9</v>
+        <v>26</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C182" t="s">
         <v>57</v>
@@ -9353,10 +9343,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>33</v>
-      </c>
-      <c r="B183" t="s">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C183" t="s">
         <v>57</v>
@@ -9364,10 +9354,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>33</v>
-      </c>
-      <c r="B184" t="s">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C184" t="s">
         <v>57</v>
@@ -9375,10 +9365,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>33</v>
-      </c>
-      <c r="B185" t="s">
-        <v>2</v>
+        <v>29</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C185" t="s">
         <v>57</v>
@@ -9386,10 +9376,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>33</v>
-      </c>
-      <c r="B186" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C186" t="s">
         <v>57</v>
@@ -9397,10 +9387,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C187" t="s">
         <v>57</v>
@@ -9408,10 +9398,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C188" t="s">
         <v>57</v>
@@ -9430,10 +9420,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C190" t="s">
         <v>57</v>
@@ -9441,10 +9431,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C191" t="s">
         <v>57</v>
@@ -9452,10 +9442,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>33</v>
-      </c>
-      <c r="B192" s="5" t="s">
-        <v>64</v>
+        <v>36</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C192" t="s">
         <v>57</v>
@@ -9463,10 +9453,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>33</v>
-      </c>
-      <c r="B193" s="5" t="s">
-        <v>65</v>
+        <v>37</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C193" t="s">
         <v>57</v>
@@ -9474,10 +9464,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>34</v>
-      </c>
-      <c r="B194" t="s">
-        <v>5</v>
+        <v>38</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C194" t="s">
         <v>57</v>
@@ -9485,10 +9475,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>34</v>
-      </c>
-      <c r="B195" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C195" t="s">
         <v>57</v>
@@ -9496,10 +9486,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>34</v>
-      </c>
-      <c r="B196" t="s">
-        <v>7</v>
+        <v>40</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C196" t="s">
         <v>57</v>
@@ -9507,10 +9497,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>34</v>
-      </c>
-      <c r="B197" t="s">
-        <v>8</v>
+        <v>41</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C197" t="s">
         <v>57</v>
@@ -9518,10 +9508,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>34</v>
-      </c>
-      <c r="B198" t="s">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C198" t="s">
         <v>57</v>
@@ -9529,10 +9519,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>34</v>
-      </c>
-      <c r="B199" t="s">
-        <v>4</v>
+        <v>43</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C199" t="s">
         <v>57</v>
@@ -9540,21 +9530,21 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B200" t="s">
         <v>1</v>
       </c>
       <c r="C200" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B201" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C201" t="s">
         <v>57</v>
@@ -9562,10 +9552,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B202" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C202" t="s">
         <v>57</v>
@@ -9573,10 +9563,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>34</v>
-      </c>
-      <c r="B203" s="6" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1</v>
       </c>
       <c r="C203" t="s">
         <v>57</v>
@@ -9584,10 +9574,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>34</v>
-      </c>
-      <c r="B204" s="6" t="s">
-        <v>60</v>
+        <v>26</v>
+      </c>
+      <c r="B204" t="s">
+        <v>1</v>
       </c>
       <c r="C204" t="s">
         <v>57</v>
@@ -9595,10 +9585,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>34</v>
-      </c>
-      <c r="B205" s="6" t="s">
-        <v>61</v>
+        <v>27</v>
+      </c>
+      <c r="B205" t="s">
+        <v>1</v>
       </c>
       <c r="C205" t="s">
         <v>57</v>
@@ -9606,10 +9596,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>34</v>
-      </c>
-      <c r="B206" s="6" t="s">
-        <v>63</v>
+        <v>28</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1</v>
       </c>
       <c r="C206" t="s">
         <v>57</v>
@@ -9617,10 +9607,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>34</v>
-      </c>
-      <c r="B207" s="6" t="s">
-        <v>62</v>
+        <v>29</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1</v>
       </c>
       <c r="C207" t="s">
         <v>57</v>
@@ -9628,10 +9618,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>34</v>
-      </c>
-      <c r="B208" s="5" t="s">
-        <v>64</v>
+        <v>30</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1</v>
       </c>
       <c r="C208" t="s">
         <v>57</v>
@@ -9639,10 +9629,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>34</v>
-      </c>
-      <c r="B209" s="5" t="s">
-        <v>65</v>
+        <v>31</v>
+      </c>
+      <c r="B209" t="s">
+        <v>1</v>
       </c>
       <c r="C209" t="s">
         <v>57</v>
@@ -9650,10 +9640,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B210" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C210" t="s">
         <v>57</v>
@@ -9661,10 +9651,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B211" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C211" t="s">
         <v>57</v>
@@ -9672,10 +9662,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B212" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C212" t="s">
         <v>57</v>
@@ -9686,7 +9676,7 @@
         <v>35</v>
       </c>
       <c r="B213" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C213" t="s">
         <v>57</v>
@@ -9694,10 +9684,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B214" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C214" t="s">
         <v>57</v>
@@ -9705,10 +9695,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B215" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C215" t="s">
         <v>57</v>
@@ -9716,7 +9706,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B216" t="s">
         <v>1</v>
@@ -9727,10 +9717,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B217" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C217" t="s">
         <v>57</v>
@@ -9738,10 +9728,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B218" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C218" t="s">
         <v>57</v>
@@ -9749,10 +9739,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>35</v>
-      </c>
-      <c r="B219" s="6" t="s">
-        <v>59</v>
+        <v>41</v>
+      </c>
+      <c r="B219" t="s">
+        <v>1</v>
       </c>
       <c r="C219" t="s">
         <v>57</v>
@@ -9760,10 +9750,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>35</v>
-      </c>
-      <c r="B220" s="6" t="s">
-        <v>60</v>
+        <v>42</v>
+      </c>
+      <c r="B220" t="s">
+        <v>1</v>
       </c>
       <c r="C220" t="s">
         <v>57</v>
@@ -9771,10 +9761,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>35</v>
-      </c>
-      <c r="B221" s="6" t="s">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="B221" t="s">
+        <v>1</v>
       </c>
       <c r="C221" t="s">
         <v>57</v>
@@ -9782,21 +9772,21 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>35</v>
-      </c>
-      <c r="B222" s="6" t="s">
-        <v>63</v>
+        <v>19</v>
+      </c>
+      <c r="B222" t="s">
+        <v>2</v>
       </c>
       <c r="C222" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>35</v>
-      </c>
-      <c r="B223" s="6" t="s">
-        <v>62</v>
+        <v>15</v>
+      </c>
+      <c r="B223" t="s">
+        <v>2</v>
       </c>
       <c r="C223" t="s">
         <v>57</v>
@@ -9804,10 +9794,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>35</v>
-      </c>
-      <c r="B224" s="5" t="s">
-        <v>64</v>
+        <v>24</v>
+      </c>
+      <c r="B224" t="s">
+        <v>2</v>
       </c>
       <c r="C224" t="s">
         <v>57</v>
@@ -9815,10 +9805,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>35</v>
-      </c>
-      <c r="B225" s="5" t="s">
-        <v>65</v>
+        <v>25</v>
+      </c>
+      <c r="B225" t="s">
+        <v>2</v>
       </c>
       <c r="C225" t="s">
         <v>57</v>
@@ -9826,10 +9816,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B226" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C226" t="s">
         <v>57</v>
@@ -9837,10 +9827,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B227" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C227" t="s">
         <v>57</v>
@@ -9848,10 +9838,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B228" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C228" t="s">
         <v>57</v>
@@ -9859,10 +9849,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B229" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C229" t="s">
         <v>57</v>
@@ -9870,10 +9860,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B230" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C230" t="s">
         <v>57</v>
@@ -9881,10 +9871,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B231" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C231" t="s">
         <v>57</v>
@@ -9892,10 +9882,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B232" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C232" t="s">
         <v>57</v>
@@ -9903,7 +9893,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B233" t="s">
         <v>2</v>
@@ -9914,10 +9904,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B234" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C234" t="s">
         <v>57</v>
@@ -9925,10 +9915,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>36</v>
-      </c>
-      <c r="B235" s="6" t="s">
-        <v>59</v>
+        <v>35</v>
+      </c>
+      <c r="B235" t="s">
+        <v>2</v>
       </c>
       <c r="C235" t="s">
         <v>57</v>
@@ -9938,8 +9928,8 @@
       <c r="A236" t="s">
         <v>36</v>
       </c>
-      <c r="B236" s="6" t="s">
-        <v>60</v>
+      <c r="B236" t="s">
+        <v>2</v>
       </c>
       <c r="C236" t="s">
         <v>57</v>
@@ -9947,10 +9937,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>36</v>
-      </c>
-      <c r="B237" s="6" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="B237" t="s">
+        <v>2</v>
       </c>
       <c r="C237" t="s">
         <v>57</v>
@@ -9958,10 +9948,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>36</v>
-      </c>
-      <c r="B238" s="6" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="B238" t="s">
+        <v>2</v>
       </c>
       <c r="C238" t="s">
         <v>57</v>
@@ -9969,10 +9959,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>36</v>
-      </c>
-      <c r="B239" s="6" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="B239" t="s">
+        <v>2</v>
       </c>
       <c r="C239" t="s">
         <v>57</v>
@@ -9980,10 +9970,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>36</v>
-      </c>
-      <c r="B240" s="5" t="s">
-        <v>64</v>
+        <v>40</v>
+      </c>
+      <c r="B240" t="s">
+        <v>2</v>
       </c>
       <c r="C240" t="s">
         <v>57</v>
@@ -9991,10 +9981,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>36</v>
-      </c>
-      <c r="B241" s="5" t="s">
-        <v>65</v>
+        <v>41</v>
+      </c>
+      <c r="B241" t="s">
+        <v>2</v>
       </c>
       <c r="C241" t="s">
         <v>57</v>
@@ -10002,10 +9992,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B242" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C242" t="s">
         <v>57</v>
@@ -10013,10 +10003,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B243" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C243" t="s">
         <v>57</v>
@@ -10024,21 +10014,21 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B244" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C244" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B245" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C245" t="s">
         <v>57</v>
@@ -10046,10 +10036,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B246" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C246" t="s">
         <v>57</v>
@@ -10057,10 +10047,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B247" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C247" t="s">
         <v>57</v>
@@ -10068,10 +10058,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B248" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C248" t="s">
         <v>57</v>
@@ -10079,10 +10069,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B249" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C249" t="s">
         <v>57</v>
@@ -10090,7 +10080,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B250" t="s">
         <v>3</v>
@@ -10101,10 +10091,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>37</v>
-      </c>
-      <c r="B251" s="6" t="s">
-        <v>59</v>
+        <v>29</v>
+      </c>
+      <c r="B251" t="s">
+        <v>3</v>
       </c>
       <c r="C251" t="s">
         <v>57</v>
@@ -10112,10 +10102,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>37</v>
-      </c>
-      <c r="B252" s="6" t="s">
-        <v>60</v>
+        <v>30</v>
+      </c>
+      <c r="B252" t="s">
+        <v>3</v>
       </c>
       <c r="C252" t="s">
         <v>57</v>
@@ -10123,10 +10113,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>37</v>
-      </c>
-      <c r="B253" s="6" t="s">
-        <v>61</v>
+        <v>31</v>
+      </c>
+      <c r="B253" t="s">
+        <v>3</v>
       </c>
       <c r="C253" t="s">
         <v>57</v>
@@ -10134,10 +10124,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>37</v>
-      </c>
-      <c r="B254" s="6" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="B254" t="s">
+        <v>3</v>
       </c>
       <c r="C254" t="s">
         <v>57</v>
@@ -10145,10 +10135,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>37</v>
-      </c>
-      <c r="B255" s="6" t="s">
-        <v>62</v>
+        <v>33</v>
+      </c>
+      <c r="B255" t="s">
+        <v>3</v>
       </c>
       <c r="C255" t="s">
         <v>57</v>
@@ -10156,10 +10146,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>37</v>
-      </c>
-      <c r="B256" s="5" t="s">
-        <v>64</v>
+        <v>34</v>
+      </c>
+      <c r="B256" t="s">
+        <v>3</v>
       </c>
       <c r="C256" t="s">
         <v>57</v>
@@ -10167,10 +10157,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>37</v>
-      </c>
-      <c r="B257" s="5" t="s">
-        <v>65</v>
+        <v>35</v>
+      </c>
+      <c r="B257" t="s">
+        <v>3</v>
       </c>
       <c r="C257" t="s">
         <v>57</v>
@@ -10178,10 +10168,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B258" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C258" t="s">
         <v>57</v>
@@ -10189,10 +10179,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B259" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C259" t="s">
         <v>57</v>
@@ -10203,7 +10193,7 @@
         <v>38</v>
       </c>
       <c r="B260" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C260" t="s">
         <v>57</v>
@@ -10211,10 +10201,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B261" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C261" t="s">
         <v>57</v>
@@ -10222,10 +10212,10 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B262" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C262" t="s">
         <v>57</v>
@@ -10233,10 +10223,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B263" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C263" t="s">
         <v>57</v>
@@ -10244,10 +10234,10 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B264" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C264" t="s">
         <v>57</v>
@@ -10255,10 +10245,10 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B265" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C265" t="s">
         <v>57</v>
@@ -10266,21 +10256,21 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>38</v>
-      </c>
-      <c r="B266" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="B266" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C266" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B267" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C267" t="s">
         <v>57</v>
@@ -10288,10 +10278,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B268" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C268" t="s">
         <v>57</v>
@@ -10299,10 +10289,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B269" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C269" t="s">
         <v>57</v>
@@ -10310,7 +10300,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B270" s="6" t="s">
         <v>63</v>
@@ -10321,10 +10311,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C271" t="s">
         <v>57</v>
@@ -10332,161 +10322,163 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>28</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C272" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>29</v>
+      </c>
+      <c r="B273" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C273" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>30</v>
+      </c>
+      <c r="B274" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C274" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>31</v>
+      </c>
+      <c r="B275" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C275" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>32</v>
+      </c>
+      <c r="B276" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C276" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>33</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C277" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>34</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C278" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>35</v>
+      </c>
+      <c r="B279" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C279" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>36</v>
+      </c>
+      <c r="B280" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C280" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>37</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C281" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
         <v>38</v>
       </c>
-      <c r="B272" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C272" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>38</v>
-      </c>
-      <c r="B273" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C273" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>39</v>
-      </c>
-      <c r="B274" t="s">
-        <v>5</v>
-      </c>
-      <c r="C274" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>39</v>
-      </c>
-      <c r="B275" t="s">
-        <v>6</v>
-      </c>
-      <c r="C275" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>39</v>
-      </c>
-      <c r="B276" t="s">
-        <v>7</v>
-      </c>
-      <c r="C276" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>39</v>
-      </c>
-      <c r="B277" t="s">
-        <v>8</v>
-      </c>
-      <c r="C277" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>39</v>
-      </c>
-      <c r="B278" t="s">
-        <v>9</v>
-      </c>
-      <c r="C278" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>39</v>
-      </c>
-      <c r="B279" t="s">
-        <v>4</v>
-      </c>
-      <c r="C279" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>39</v>
-      </c>
-      <c r="B280" t="s">
-        <v>1</v>
-      </c>
-      <c r="C280" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>39</v>
-      </c>
-      <c r="B281" t="s">
-        <v>2</v>
-      </c>
-      <c r="C281" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>39</v>
-      </c>
-      <c r="B282" t="s">
-        <v>3</v>
+      <c r="B282" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C282" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>39</v>
       </c>
       <c r="B283" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C283" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F283" s="5"/>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B284" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C284" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F284" s="5"/>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B285" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C285" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B286" s="6" t="s">
         <v>63</v>
@@ -10495,34 +10487,34 @@
         <v>57</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B287" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C287" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>19</v>
+      </c>
+      <c r="B288" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C287" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>39</v>
-      </c>
-      <c r="B288" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="C288" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>39</v>
-      </c>
-      <c r="B289" s="5" t="s">
-        <v>65</v>
+        <v>15</v>
+      </c>
+      <c r="B289" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C289" t="s">
         <v>57</v>
@@ -10530,10 +10522,10 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>40</v>
-      </c>
-      <c r="B290" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C290" t="s">
         <v>57</v>
@@ -10541,10 +10533,10 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>40</v>
-      </c>
-      <c r="B291" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C291" t="s">
         <v>57</v>
@@ -10552,10 +10544,10 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>40</v>
-      </c>
-      <c r="B292" t="s">
-        <v>7</v>
+        <v>26</v>
+      </c>
+      <c r="B292" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C292" t="s">
         <v>57</v>
@@ -10563,10 +10555,10 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>40</v>
-      </c>
-      <c r="B293" t="s">
-        <v>8</v>
+        <v>27</v>
+      </c>
+      <c r="B293" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C293" t="s">
         <v>57</v>
@@ -10574,10 +10566,10 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>40</v>
-      </c>
-      <c r="B294" t="s">
-        <v>9</v>
+        <v>28</v>
+      </c>
+      <c r="B294" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C294" t="s">
         <v>57</v>
@@ -10585,10 +10577,10 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>40</v>
-      </c>
-      <c r="B295" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="B295" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C295" t="s">
         <v>57</v>
@@ -10596,10 +10588,10 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>40</v>
-      </c>
-      <c r="B296" t="s">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C296" t="s">
         <v>57</v>
@@ -10607,10 +10599,10 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>40</v>
-      </c>
-      <c r="B297" t="s">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C297" t="s">
         <v>57</v>
@@ -10618,10 +10610,10 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>40</v>
-      </c>
-      <c r="B298" t="s">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C298" t="s">
         <v>57</v>
@@ -10629,10 +10621,10 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B299" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C299" t="s">
         <v>57</v>
@@ -10640,10 +10632,10 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B300" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C300" t="s">
         <v>57</v>
@@ -10651,10 +10643,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B301" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C301" t="s">
         <v>57</v>
@@ -10662,10 +10654,10 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B302" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C302" t="s">
         <v>57</v>
@@ -10673,7 +10665,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B303" s="6" t="s">
         <v>62</v>
@@ -10684,560 +10676,74 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
+        <v>38</v>
+      </c>
+      <c r="B304" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C304" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>39</v>
+      </c>
+      <c r="B305" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C305" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
         <v>40</v>
       </c>
-      <c r="B304" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C304" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
-        <v>40</v>
-      </c>
-      <c r="B305" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C305" t="s">
-        <v>57</v>
-      </c>
-      <c r="F305" s="5"/>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
-        <v>41</v>
-      </c>
-      <c r="B306" t="s">
-        <v>5</v>
+      <c r="B306" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C306" t="s">
         <v>57</v>
       </c>
-      <c r="F306" s="5"/>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>41</v>
       </c>
-      <c r="B307" t="s">
-        <v>6</v>
+      <c r="B307" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C307" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>41</v>
-      </c>
-      <c r="B308" t="s">
-        <v>7</v>
+        <v>42</v>
+      </c>
+      <c r="B308" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C308" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>41</v>
-      </c>
-      <c r="B309" t="s">
-        <v>8</v>
+        <v>43</v>
+      </c>
+      <c r="B309" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C309" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
-        <v>41</v>
-      </c>
-      <c r="B310" t="s">
-        <v>9</v>
-      </c>
-      <c r="C310" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
-        <v>41</v>
-      </c>
-      <c r="B311" t="s">
-        <v>4</v>
-      </c>
-      <c r="C311" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>41</v>
-      </c>
-      <c r="B312" t="s">
-        <v>1</v>
-      </c>
-      <c r="C312" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
-        <v>41</v>
-      </c>
-      <c r="B313" t="s">
-        <v>2</v>
-      </c>
-      <c r="C313" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
-        <v>41</v>
-      </c>
-      <c r="B314" t="s">
-        <v>3</v>
-      </c>
-      <c r="C314" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
-        <v>41</v>
-      </c>
-      <c r="B315" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C315" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
-        <v>41</v>
-      </c>
-      <c r="B316" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C316" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
-        <v>41</v>
-      </c>
-      <c r="B317" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C317" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
-        <v>41</v>
-      </c>
-      <c r="B318" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C318" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A319" t="s">
-        <v>41</v>
-      </c>
-      <c r="B319" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C319" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
-        <v>41</v>
-      </c>
-      <c r="B320" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C320" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
-        <v>41</v>
-      </c>
-      <c r="B321" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C321" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
-        <v>42</v>
-      </c>
-      <c r="B322" t="s">
-        <v>5</v>
-      </c>
-      <c r="C322" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
-        <v>42</v>
-      </c>
-      <c r="B323" t="s">
-        <v>6</v>
-      </c>
-      <c r="C323" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A324" t="s">
-        <v>42</v>
-      </c>
-      <c r="B324" t="s">
-        <v>7</v>
-      </c>
-      <c r="C324" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
-        <v>42</v>
-      </c>
-      <c r="B325" t="s">
-        <v>8</v>
-      </c>
-      <c r="C325" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
-        <v>42</v>
-      </c>
-      <c r="B326" t="s">
-        <v>9</v>
-      </c>
-      <c r="C326" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>42</v>
-      </c>
-      <c r="B327" t="s">
-        <v>4</v>
-      </c>
-      <c r="C327" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
-        <v>42</v>
-      </c>
-      <c r="B328" t="s">
-        <v>1</v>
-      </c>
-      <c r="C328" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
-        <v>42</v>
-      </c>
-      <c r="B329" t="s">
-        <v>2</v>
-      </c>
-      <c r="C329" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
-        <v>42</v>
-      </c>
-      <c r="B330" t="s">
-        <v>3</v>
-      </c>
-      <c r="C330" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
-        <v>42</v>
-      </c>
-      <c r="B331" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C331" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>42</v>
-      </c>
-      <c r="B332" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C332" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
-        <v>42</v>
-      </c>
-      <c r="B333" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C333" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
-        <v>42</v>
-      </c>
-      <c r="B334" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C334" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
-        <v>42</v>
-      </c>
-      <c r="B335" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C335" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A336" t="s">
-        <v>42</v>
-      </c>
-      <c r="B336" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C336" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
-        <v>42</v>
-      </c>
-      <c r="B337" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C337" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
-        <v>43</v>
-      </c>
-      <c r="B338" t="s">
-        <v>5</v>
-      </c>
-      <c r="C338" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
-        <v>43</v>
-      </c>
-      <c r="B339" t="s">
-        <v>6</v>
-      </c>
-      <c r="C339" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A340" t="s">
-        <v>43</v>
-      </c>
-      <c r="B340" t="s">
-        <v>7</v>
-      </c>
-      <c r="C340" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
-        <v>43</v>
-      </c>
-      <c r="B341" t="s">
-        <v>8</v>
-      </c>
-      <c r="C341" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
-        <v>43</v>
-      </c>
-      <c r="B342" t="s">
-        <v>9</v>
-      </c>
-      <c r="C342" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
-        <v>43</v>
-      </c>
-      <c r="B343" t="s">
-        <v>4</v>
-      </c>
-      <c r="C343" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
-        <v>43</v>
-      </c>
-      <c r="B344" t="s">
-        <v>1</v>
-      </c>
-      <c r="C344" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
-        <v>43</v>
-      </c>
-      <c r="B345" t="s">
-        <v>2</v>
-      </c>
-      <c r="C345" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
-        <v>43</v>
-      </c>
-      <c r="B346" t="s">
-        <v>3</v>
-      </c>
-      <c r="C346" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
-        <v>43</v>
-      </c>
-      <c r="B347" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C347" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
-        <v>43</v>
-      </c>
-      <c r="B348" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C348" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
-        <v>43</v>
-      </c>
-      <c r="B349" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C349" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
-        <v>43</v>
-      </c>
-      <c r="B350" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C350" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
-        <v>43</v>
-      </c>
-      <c r="B351" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C351" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>43</v>
-      </c>
-      <c r="B352" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C352" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
-        <v>43</v>
-      </c>
-      <c r="B353" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C353" t="s">
-        <v>57</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C353" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C353">
-      <sortCondition ref="A1:A353"/>
+  <autoFilter ref="A1:C309" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C309">
+      <sortCondition ref="B1:B309"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>